<commit_message>
started generator in aws main gen
</commit_message>
<xml_diff>
--- a/corpus_movies_list.xlsx
+++ b/corpus_movies_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rohit Suresh\Jupyter projects\Plot summary generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2247794-BB1D-414A-BDBF-2FC4A8B6FF9B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57C3AC4A-3C86-480F-AF38-0A5E929D548F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="119">
   <si>
     <t>wikipedia page title</t>
   </si>
@@ -160,22 +160,236 @@
   </si>
   <si>
     <t>imdb id</t>
+  </si>
+  <si>
+    <t>Captain America (serial)</t>
+  </si>
+  <si>
+    <t>tt0036697</t>
+  </si>
+  <si>
+    <t>tt0091225</t>
+  </si>
+  <si>
+    <t>Howard the Duck (film)</t>
+  </si>
+  <si>
+    <t>The Punisher (1989 film)</t>
+  </si>
+  <si>
+    <t>tt0098141</t>
+  </si>
+  <si>
+    <t>Captain America (1990 film)</t>
+  </si>
+  <si>
+    <t>tt0103923</t>
+  </si>
+  <si>
+    <t>tt0120611</t>
+  </si>
+  <si>
+    <t>Blade II</t>
+  </si>
+  <si>
+    <t>Spider-Man 2</t>
+  </si>
+  <si>
+    <t>Blade: Trinity</t>
+  </si>
+  <si>
+    <t>X-Men: The Last Stand</t>
+  </si>
+  <si>
+    <t>Fantastic Four: Rise of the Silver Surfer</t>
+  </si>
+  <si>
+    <t>Punisher: War Zone</t>
+  </si>
+  <si>
+    <t>X-Men Origins: Wolverine</t>
+  </si>
+  <si>
+    <t>X-Men: First Class</t>
+  </si>
+  <si>
+    <t>Ghost Rider: Spirit of Vengeance</t>
+  </si>
+  <si>
+    <t>The Amazing Spider-Man 2</t>
+  </si>
+  <si>
+    <t>X-Men: Days of Future Past</t>
+  </si>
+  <si>
+    <t>X-Men: Apocalypse</t>
+  </si>
+  <si>
+    <t>Deadpool 2</t>
+  </si>
+  <si>
+    <t>Spider-Man: Far From Home</t>
+  </si>
+  <si>
+    <t>Blade (film)</t>
+  </si>
+  <si>
+    <t>X-Men (film)</t>
+  </si>
+  <si>
+    <t>Spider-Man (2002 film)</t>
+  </si>
+  <si>
+    <t>Daredevil (film)</t>
+  </si>
+  <si>
+    <t>X2 (film)</t>
+  </si>
+  <si>
+    <t>Hulk (film)</t>
+  </si>
+  <si>
+    <t>The Punisher (2004 film)</t>
+  </si>
+  <si>
+    <t>Elektra (2005 film)</t>
+  </si>
+  <si>
+    <t>Fantastic Four (2005 film)</t>
+  </si>
+  <si>
+    <t>Ghost Rider (2007 film)</t>
+  </si>
+  <si>
+    <t>The Amazing Spider-Man (2012 film)</t>
+  </si>
+  <si>
+    <t>The Wolverine (film)</t>
+  </si>
+  <si>
+    <t>Fantastic Four (2015 film)</t>
+  </si>
+  <si>
+    <t>Deadpool (film)</t>
+  </si>
+  <si>
+    <t>Logan (film)</t>
+  </si>
+  <si>
+    <t>Venom (2018 film)</t>
+  </si>
+  <si>
+    <t>Dark Phoenix (film)</t>
+  </si>
+  <si>
+    <t>tt0120903</t>
+  </si>
+  <si>
+    <t>tt3385516</t>
+  </si>
+  <si>
+    <t>tt1270798</t>
+  </si>
+  <si>
+    <t>tt0458525</t>
+  </si>
+  <si>
+    <t>tt0376994</t>
+  </si>
+  <si>
+    <t>tt0290334</t>
+  </si>
+  <si>
+    <t>tt1877832</t>
+  </si>
+  <si>
+    <t>tt6565702</t>
+  </si>
+  <si>
+    <t>tt0187738</t>
+  </si>
+  <si>
+    <t>tt0359013</t>
+  </si>
+  <si>
+    <t>tt0145487</t>
+  </si>
+  <si>
+    <t>tt0948470</t>
+  </si>
+  <si>
+    <t>tt1872181</t>
+  </si>
+  <si>
+    <t>tt6320628</t>
+  </si>
+  <si>
+    <t>tt0316654</t>
+  </si>
+  <si>
+    <t>Spider-Man 3</t>
+  </si>
+  <si>
+    <t>tt0413300</t>
+  </si>
+  <si>
+    <t>Spider-Man: Into the Spider-Verse</t>
+  </si>
+  <si>
+    <t>tt4633694</t>
+  </si>
+  <si>
+    <t>tt0287978</t>
+  </si>
+  <si>
+    <t>tt0286716</t>
+  </si>
+  <si>
+    <t>tt0330793</t>
+  </si>
+  <si>
+    <t>tt0450314</t>
+  </si>
+  <si>
+    <t>tt0357277</t>
+  </si>
+  <si>
+    <t>tt0120667</t>
+  </si>
+  <si>
+    <t>tt0486576</t>
+  </si>
+  <si>
+    <t>tt1502712</t>
+  </si>
+  <si>
+    <t>tt0259324</t>
+  </si>
+  <si>
+    <t>tt1071875</t>
+  </si>
+  <si>
+    <t>tt1430132</t>
+  </si>
+  <si>
+    <t>tt3315342</t>
+  </si>
+  <si>
+    <t>tt1431045</t>
+  </si>
+  <si>
+    <t>tt5463162</t>
+  </si>
+  <si>
+    <t>tt1270797</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -225,18 +439,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -517,275 +734,679 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:C60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14" style="3" customWidth="1"/>
-    <col min="2" max="2" width="45" style="4" customWidth="1"/>
-    <col min="3" max="3" width="11.77734375" style="3" customWidth="1"/>
-    <col min="4" max="16384" width="8.88671875" style="3"/>
+    <col min="1" max="1" width="14" style="7" customWidth="1"/>
+    <col min="2" max="2" width="45" style="2" customWidth="1"/>
+    <col min="3" max="3" width="11.77734375" style="7" customWidth="1"/>
+    <col min="4" max="16384" width="8.88671875" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="6" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="3">
+      <c r="A2" s="7">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="7" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="3">
+      <c r="A3" s="7">
         <v>2</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="7" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="3">
+      <c r="A4" s="7">
         <v>3</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="7" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="3">
+      <c r="A5" s="7">
         <v>4</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="7" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="3">
+      <c r="A6" s="7">
         <v>5</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="7" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="3">
+      <c r="A7" s="7">
         <v>6</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="7" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="3">
+      <c r="A8" s="7">
         <v>7</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="7" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="3">
+      <c r="A9" s="7">
         <v>8</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="7" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="3">
+      <c r="A10" s="7">
         <v>9</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="7" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="3">
+      <c r="A11" s="7">
         <v>10</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="7" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="3">
+      <c r="A12" s="7">
         <v>11</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="7" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="3">
+      <c r="A13" s="7">
         <v>12</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="7" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="3">
+      <c r="A14" s="7">
         <v>13</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="7" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="3">
+      <c r="A15" s="7">
         <v>14</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="7" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="3">
+      <c r="A16" s="7">
         <v>15</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="7" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="3">
+      <c r="A17" s="7">
         <v>16</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="7" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="3">
+      <c r="A18" s="7">
         <v>17</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" s="7" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="3">
+      <c r="A19" s="7">
         <v>18</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" s="7" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="3">
+      <c r="A20" s="7">
         <v>19</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" s="7" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="3">
+      <c r="A21" s="7">
         <v>20</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B21" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C21" s="7" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="3">
+      <c r="A22" s="7">
         <v>21</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="B22" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C22" s="7" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="3">
+      <c r="A23" s="7">
         <v>22</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="B23" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C23" s="7" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B24" s="5"/>
+      <c r="A24" s="7">
+        <v>23</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="7">
+        <v>24</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="7">
+        <v>25</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="7">
+        <v>26</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="7">
+        <v>27</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="7">
+        <v>28</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="7">
+        <v>29</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="7">
+        <v>30</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="7">
+        <v>31</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" s="7">
+        <v>32</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" s="7">
+        <v>33</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" s="7">
+        <v>34</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" s="7">
+        <v>35</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" s="7">
+        <v>36</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" s="7">
+        <v>37</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C38" s="7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" s="7">
+        <v>38</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" s="7">
+        <v>39</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C40" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" s="7">
+        <v>40</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" s="7">
+        <v>41</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C42" s="7" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" s="7">
+        <v>42</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" s="7">
+        <v>43</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C44" s="7" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45" s="7">
+        <v>44</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C45" s="7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46" s="7">
+        <v>45</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C46" s="7" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A47" s="7">
+        <v>46</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C47" s="7" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A48" s="7">
+        <v>47</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C48" s="7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49" s="7">
+        <v>48</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C49" s="7" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A50" s="7">
+        <v>49</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C50" s="7" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51" s="7">
+        <v>50</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C51" s="7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52" s="7">
+        <v>51</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C52" s="7" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A53" s="7">
+        <v>52</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C53" s="7" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A54" s="7">
+        <v>53</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C54" s="7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A55" s="7">
+        <v>54</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C55" s="7" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A56" s="7">
+        <v>55</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C56" s="7" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A57" s="7">
+        <v>56</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C57" s="7" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A58" s="7">
+        <v>57</v>
+      </c>
+      <c r="B58" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C58" s="7" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A59" s="7">
+        <v>58</v>
+      </c>
+      <c r="B59" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C59" s="7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A60" s="7">
+        <v>59</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C60" s="7" t="s">
+        <v>103</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>